<commit_message>
Parę sprawozdanek i chuj wi jakie
</commit_message>
<xml_diff>
--- a/Fizyka/Fizyka/Lab 8 A1/Zeszyt1.xlsx
+++ b/Fizyka/Fizyka/Lab 8 A1/Zeszyt1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RedScorp\Desktop\Sprawozdania\Fizyka\Fizyka\Lab 8 A1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4BDAB4E5-CCF4-463A-BAD3-1A1C6E2227F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EACD3D6A-10FB-44E5-8904-852B85C9468B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13875" xr2:uid="{3C928035-6354-4E13-993B-229068EF3C69}"/>
+    <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="21600" xr2:uid="{3C928035-6354-4E13-993B-229068EF3C69}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -20,23 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="28">
   <si>
     <t>Lp.</t>
   </si>
@@ -96,6 +85,30 @@
   </si>
   <si>
     <t>λ - 3 kHz [m]</t>
+  </si>
+  <si>
+    <t>U(λ)</t>
+  </si>
+  <si>
+    <t>U(υ)</t>
+  </si>
+  <si>
+    <t>1,3 ± 1,6E-02 m</t>
+  </si>
+  <si>
+    <t>0,90 ± 1,6E-02 m</t>
+  </si>
+  <si>
+    <t>1,2 ± 1,6E-02 m</t>
+  </si>
+  <si>
+    <t>331 ± 4,1 m/s</t>
+  </si>
+  <si>
+    <t>246 ± 4,5 m/s</t>
+  </si>
+  <si>
+    <t>352 ± 4,9 m/s</t>
   </si>
 </sst>
 </file>
@@ -103,8 +116,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="169" formatCode="0.0E+00"/>
-    <numFmt numFmtId="172" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0E+00"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -123,7 +136,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -145,6 +158,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -189,23 +208,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -227,13 +248,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>80963</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>514368</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>90515</xdr:rowOff>
@@ -569,53 +590,53 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{321CC485-B4F2-47E7-ADD5-A819AB11FBAF}">
-  <dimension ref="B1:L38"/>
+  <dimension ref="B1:M38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="J32" sqref="J32"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="10.86328125" customWidth="1"/>
-    <col min="4" max="4" width="10.9296875" customWidth="1"/>
-    <col min="5" max="5" width="11.1328125" customWidth="1"/>
-    <col min="6" max="6" width="11.46484375" customWidth="1"/>
-    <col min="7" max="7" width="11.53125" customWidth="1"/>
-    <col min="8" max="8" width="11.3984375" customWidth="1"/>
-    <col min="10" max="10" width="13.796875" customWidth="1"/>
-    <col min="11" max="11" width="16.1328125" customWidth="1"/>
-    <col min="12" max="12" width="13.19921875" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" customWidth="1"/>
+    <col min="4" max="4" width="11" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" customWidth="1"/>
+    <col min="11" max="11" width="13.85546875" customWidth="1"/>
+    <col min="12" max="12" width="16.140625" customWidth="1"/>
+    <col min="13" max="13" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" x14ac:dyDescent="0.45">
-      <c r="B1" s="7" t="s">
+    <row r="1" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6" t="s">
+      <c r="D1" s="9"/>
+      <c r="E1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6" t="s">
+      <c r="F1" s="9"/>
+      <c r="G1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="6"/>
-      <c r="J1" s="3" t="s">
+      <c r="H1" s="9"/>
+      <c r="K1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="L1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="M1" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.45">
-      <c r="B2" s="7"/>
+    <row r="2" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B2" s="10"/>
       <c r="C2" s="1" t="s">
         <v>11</v>
       </c>
@@ -634,20 +655,20 @@
       <c r="H2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J2" s="11">
+      <c r="K2" s="8">
         <f>2*ABS(D13-C13)</f>
         <v>1.3219999999999996</v>
       </c>
-      <c r="K2" s="10">
+      <c r="L2" s="7">
         <f>2*ABS(F13-E13)</f>
         <v>0.89600000000000035</v>
       </c>
-      <c r="L2" s="11">
+      <c r="M2" s="8">
         <f>2*ABS(H13-G13)</f>
         <v>1.1740000000000002</v>
       </c>
     </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B3" s="1">
         <v>1</v>
       </c>
@@ -670,16 +691,22 @@
         <v>0.79</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="K3" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="L3" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.45">
+        <v>20</v>
+      </c>
+      <c r="K3" s="6">
+        <f>SQRT(((2*C13-2*D13)/(ABS(C13-D13)) * C38)^2+((2*D13-2*C13)/(ABS(D13-C13)) * D38)^2)</f>
+        <v>1.6337741290311087E-2</v>
+      </c>
+      <c r="L3" s="6">
+        <f>SQRT(((2*E13-2*F13)/(ABS(E13-F13)) * E38)^2+((2*F13-2*E13)/(ABS(F13-E13)) * F38)^2)</f>
+        <v>1.641085061404628E-2</v>
+      </c>
+      <c r="M3" s="6">
+        <f>SQRT(((2*G13-2*H13)/(ABS(G13-H13)) * G38)^2+((2*H13-2*G13)/(ABS(H13-G13)) * H38)^2)</f>
+        <v>1.6333536387248791E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B4" s="1">
         <v>2</v>
       </c>
@@ -701,66 +728,84 @@
       <c r="H4" s="2">
         <v>0.88</v>
       </c>
-      <c r="J4" s="2">
+      <c r="K4" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="L4" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="M4" s="12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B5" s="1">
+        <v>3</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="D5" s="2">
+        <v>1</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="F5" s="2">
+        <v>0.99</v>
+      </c>
+      <c r="G5" s="2">
+        <v>0.22</v>
+      </c>
+      <c r="H5" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B6" s="1">
+        <v>4</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0.27</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0.88</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0.62</v>
+      </c>
+      <c r="F6" s="2">
+        <v>0.98</v>
+      </c>
+      <c r="G6" s="2">
+        <v>0.22</v>
+      </c>
+      <c r="H6" s="2">
+        <v>0.86</v>
+      </c>
+      <c r="K6" s="11">
         <f>2*250*ABS(D13-C13)</f>
         <v>330.49999999999989</v>
       </c>
-      <c r="K4" s="2">
+      <c r="L6" s="11">
         <f>2*275*ABS(F13-E13)</f>
         <v>246.40000000000009</v>
       </c>
-      <c r="L4" s="2">
+      <c r="M6" s="11">
         <f>2*300*ABS(H13-G13)</f>
         <v>352.20000000000005</v>
       </c>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.45">
-      <c r="B5" s="1">
-        <v>3</v>
-      </c>
-      <c r="C5" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="D5" s="2">
-        <v>1</v>
-      </c>
-      <c r="E5" s="2">
-        <v>0.56000000000000005</v>
-      </c>
-      <c r="F5" s="2">
-        <v>0.99</v>
-      </c>
-      <c r="G5" s="2">
-        <v>0.22</v>
-      </c>
-      <c r="H5" s="2">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.45">
-      <c r="B6" s="1">
-        <v>4</v>
-      </c>
-      <c r="C6" s="2">
-        <v>0.27</v>
-      </c>
-      <c r="D6" s="2">
-        <v>0.88</v>
-      </c>
-      <c r="E6" s="2">
-        <v>0.62</v>
-      </c>
-      <c r="F6" s="2">
-        <v>0.98</v>
-      </c>
-      <c r="G6" s="2">
-        <v>0.22</v>
-      </c>
-      <c r="H6" s="2">
-        <v>0.86</v>
-      </c>
-    </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
         <v>5</v>
       </c>
@@ -782,8 +827,23 @@
       <c r="H7" s="2">
         <v>0.86</v>
       </c>
-    </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="J7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K7" s="8">
+        <f>SQRT(((2*250*C13-2*250*D13)/(ABS(C13-D13)) * C38)^2+((2*250*D13-2*250*C13)/(ABS(D13-C13)) * D38)^2)</f>
+        <v>4.0844353225777725</v>
+      </c>
+      <c r="L7" s="8">
+        <f>SQRT(((2*275*E13-2*275*F13)/(ABS(E13-F13)) * E38)^2+((2*275*F13-2*275*E13)/(ABS(F13-E13)) * F38)^2)</f>
+        <v>4.5129839188627274</v>
+      </c>
+      <c r="M7" s="8">
+        <f>SQRT(((600*G13-600*H13)/(ABS(G13-H13)) * G38)^2+((600*H13-600*G13)/(ABS(H13-G13)) * H38)^2)</f>
+        <v>4.9000609161746373</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
         <v>6</v>
       </c>
@@ -805,8 +865,17 @@
       <c r="H8" s="2">
         <v>0.82</v>
       </c>
-    </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="K8" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="L8" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="M8" s="12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
         <v>7</v>
       </c>
@@ -829,7 +898,7 @@
         <v>0.86</v>
       </c>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B10" s="1">
         <v>8</v>
       </c>
@@ -852,7 +921,7 @@
         <v>0.86</v>
       </c>
     </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.45">
+    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B11" s="1">
         <v>9</v>
       </c>
@@ -875,7 +944,7 @@
         <v>0.82</v>
       </c>
     </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.45">
+    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B12" s="1">
         <v>10</v>
       </c>
@@ -898,36 +967,36 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.45">
-      <c r="B13" s="8" t="s">
+    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B13" s="5" t="s">
         <v>4</v>
       </c>
       <c r="C13" s="2">
-        <f>AVERAGE(C3:C12)</f>
+        <f t="shared" ref="C13:H13" si="0">AVERAGE(C3:C12)</f>
         <v>0.25800000000000006</v>
       </c>
       <c r="D13" s="2">
-        <f>AVERAGE(D3:D12)</f>
+        <f t="shared" si="0"/>
         <v>0.91899999999999993</v>
       </c>
       <c r="E13" s="2">
-        <f>AVERAGE(E3:E12)</f>
+        <f t="shared" si="0"/>
         <v>0.59299999999999997</v>
       </c>
       <c r="F13" s="2">
-        <f>AVERAGE(F3:F12)</f>
+        <f t="shared" si="0"/>
         <v>1.0410000000000001</v>
       </c>
       <c r="G13" s="2">
-        <f>AVERAGE(G3:G12)</f>
+        <f t="shared" si="0"/>
         <v>0.25800000000000001</v>
       </c>
       <c r="H13" s="2">
-        <f>AVERAGE(H3:H12)</f>
+        <f t="shared" si="0"/>
         <v>0.84500000000000008</v>
       </c>
     </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.45">
+    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C14" s="3" t="s">
         <v>5</v>
       </c>
@@ -947,7 +1016,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.45">
+    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B15" s="1">
         <v>1</v>
       </c>
@@ -956,32 +1025,32 @@
         <v>2.8000000000000053E-2</v>
       </c>
       <c r="D15" s="2">
-        <f t="shared" ref="D15:H15" si="0">D$13-D3</f>
+        <f>D$13-D3</f>
         <v>1.8999999999999906E-2</v>
       </c>
       <c r="E15" s="2">
-        <f t="shared" si="0"/>
+        <f>E$13-E3</f>
         <v>2.300000000000002E-2</v>
       </c>
       <c r="F15" s="2">
-        <f t="shared" si="0"/>
+        <f>F$13-F3</f>
         <v>5.1000000000000156E-2</v>
       </c>
       <c r="G15" s="2">
-        <f t="shared" si="0"/>
+        <f>G$13-G3</f>
         <v>-2.200000000000002E-2</v>
       </c>
       <c r="H15" s="2">
-        <f t="shared" si="0"/>
+        <f>H$13-H3</f>
         <v>5.5000000000000049E-2</v>
       </c>
     </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.45">
+    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B16" s="1">
         <v>2</v>
       </c>
       <c r="C16" s="2">
-        <f t="shared" ref="C16:H25" si="1">C$13-C4</f>
+        <f t="shared" ref="C16:H24" si="1">C$13-C4</f>
         <v>3.8000000000000062E-2</v>
       </c>
       <c r="D16" s="2">
@@ -1005,7 +1074,7 @@
         <v>-3.499999999999992E-2</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" s="1">
         <v>3</v>
       </c>
@@ -1034,7 +1103,7 @@
         <v>-5.4999999999999938E-2</v>
       </c>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" s="1">
         <v>4</v>
       </c>
@@ -1063,7 +1132,7 @@
         <v>-1.4999999999999902E-2</v>
       </c>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" s="1">
         <v>5</v>
       </c>
@@ -1092,7 +1161,7 @@
         <v>-1.4999999999999902E-2</v>
       </c>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" s="1">
         <v>6</v>
       </c>
@@ -1121,7 +1190,7 @@
         <v>2.5000000000000133E-2</v>
       </c>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21" s="1">
         <v>7</v>
       </c>
@@ -1150,7 +1219,7 @@
         <v>-1.4999999999999902E-2</v>
       </c>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" s="1">
         <v>8</v>
       </c>
@@ -1179,7 +1248,7 @@
         <v>-1.4999999999999902E-2</v>
       </c>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" s="1">
         <v>9</v>
       </c>
@@ -1208,7 +1277,7 @@
         <v>2.5000000000000133E-2</v>
       </c>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24" s="1">
         <v>10</v>
       </c>
@@ -1237,7 +1306,7 @@
         <v>4.500000000000004E-2</v>
       </c>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C25" s="4" t="s">
         <v>7</v>
       </c>
@@ -1257,7 +1326,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B26" s="1">
         <v>1</v>
       </c>
@@ -1286,7 +1355,7 @@
         <v>3.0250000000000055E-3</v>
       </c>
     </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B27" s="1">
         <v>2</v>
       </c>
@@ -1315,7 +1384,7 @@
         <v>1.2249999999999943E-3</v>
       </c>
     </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B28" s="1">
         <v>3</v>
       </c>
@@ -1344,7 +1413,7 @@
         <v>3.024999999999993E-3</v>
       </c>
     </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B29" s="1">
         <v>4</v>
       </c>
@@ -1373,7 +1442,7 @@
         <v>2.2499999999999707E-4</v>
       </c>
     </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B30" s="1">
         <v>5</v>
       </c>
@@ -1402,7 +1471,7 @@
         <v>2.2499999999999707E-4</v>
       </c>
     </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B31" s="1">
         <v>6</v>
       </c>
@@ -1431,7 +1500,7 @@
         <v>6.2500000000000663E-4</v>
       </c>
     </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B32" s="1">
         <v>7</v>
       </c>
@@ -1460,7 +1529,7 @@
         <v>2.2499999999999707E-4</v>
       </c>
     </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B33" s="1">
         <v>8</v>
       </c>
@@ -1489,7 +1558,7 @@
         <v>2.2499999999999707E-4</v>
       </c>
     </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B34" s="1">
         <v>9</v>
       </c>
@@ -1518,7 +1587,7 @@
         <v>6.2500000000000663E-4</v>
       </c>
     </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B35" s="1">
         <v>10</v>
       </c>
@@ -1547,89 +1616,89 @@
         <v>2.0250000000000038E-3</v>
       </c>
     </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="B36" s="8" t="s">
+    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B36" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C36" s="9">
+      <c r="C36" s="6">
         <f>(SUM(C26:C35))/(90)</f>
         <v>8.8444444444444486E-5</v>
       </c>
-      <c r="D36" s="9">
+      <c r="D36" s="6">
         <f t="shared" ref="D36:H36" si="12">(SUM(D26:D35))/(90)</f>
         <v>2.3655555555555544E-4</v>
       </c>
-      <c r="E36" s="9">
+      <c r="E36" s="6">
         <f t="shared" si="12"/>
         <v>8.0111111111111041E-5</v>
       </c>
-      <c r="F36" s="9">
+      <c r="F36" s="6">
         <f t="shared" si="12"/>
         <v>8.0988888888888842E-4</v>
       </c>
-      <c r="G36" s="9">
+      <c r="G36" s="6">
         <f t="shared" si="12"/>
         <v>1.1511111111111109E-4</v>
       </c>
-      <c r="H36" s="9">
+      <c r="H36" s="6">
         <f t="shared" si="12"/>
         <v>1.2722222222222223E-4</v>
       </c>
     </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="B37" s="8" t="s">
+    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B37" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C37" s="9">
+      <c r="C37" s="6">
         <f>0.01/SQRT(3)</f>
         <v>5.773502691896258E-3</v>
       </c>
-      <c r="D37" s="9">
+      <c r="D37" s="6">
         <f t="shared" ref="D37:H37" si="13">0.01/SQRT(3)</f>
         <v>5.773502691896258E-3</v>
       </c>
-      <c r="E37" s="9">
+      <c r="E37" s="6">
         <f t="shared" si="13"/>
         <v>5.773502691896258E-3</v>
       </c>
-      <c r="F37" s="9">
+      <c r="F37" s="6">
         <f t="shared" si="13"/>
         <v>5.773502691896258E-3</v>
       </c>
-      <c r="G37" s="9">
+      <c r="G37" s="6">
         <f t="shared" si="13"/>
         <v>5.773502691896258E-3</v>
       </c>
-      <c r="H37" s="9">
+      <c r="H37" s="6">
         <f t="shared" si="13"/>
         <v>5.773502691896258E-3</v>
       </c>
     </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="B38" s="8" t="s">
+    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B38" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C38" s="9">
+      <c r="C38" s="6">
         <f>SQRT(C36^2+C37^2)</f>
         <v>5.7741800935792106E-3</v>
       </c>
-      <c r="D38" s="9">
+      <c r="D38" s="6">
         <f t="shared" ref="D38:H38" si="14">SQRT(D36^2+D37^2)</f>
         <v>5.7783468106541976E-3</v>
       </c>
-      <c r="E38" s="9">
+      <c r="E38" s="6">
         <f t="shared" si="14"/>
         <v>5.7740584620747295E-3</v>
       </c>
-      <c r="F38" s="9">
+      <c r="F38" s="6">
         <f t="shared" si="14"/>
         <v>5.8300303040103498E-3</v>
       </c>
-      <c r="G38" s="9">
+      <c r="G38" s="6">
         <f t="shared" si="14"/>
         <v>5.7746501107196592E-3</v>
       </c>
-      <c r="H38" s="9">
+      <c r="H38" s="6">
         <f t="shared" si="14"/>
         <v>5.7749042266656246E-3</v>
       </c>
@@ -1643,7 +1712,7 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>